<commit_message>
TestNG Jenkins setup second push
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>UserName</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>Abcd@1234</t>
+  </si>
+  <si>
+    <t>DONE</t>
   </si>
 </sst>
 </file>
@@ -988,7 +991,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -1016,6 +1019,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4">
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="abc@xyz.com"/>

</xml_diff>

<commit_message>
TestNG Jenkins setup third push
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -41,7 +41,7 @@
     <t>Abcd@1234</t>
   </si>
   <si>
-    <t>DONE</t>
+    <t>Completed</t>
   </si>
 </sst>
 </file>
@@ -991,7 +991,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -1018,9 +1018,7 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="C4" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>